<commit_message>
edit option merge option and more
</commit_message>
<xml_diff>
--- a/examples/Book.xlsx
+++ b/examples/Book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\autoarendt\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA9EFAF-51DB-4CD1-B309-7A61E4F5EB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AFE74A-E7C0-4D9D-9191-D652A7E206A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FE36834-C715-4EC5-9DBC-D6A3CBE78FFA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>##A##</t>
   </si>
@@ -60,13 +60,41 @@
   </si>
   <si>
     <t>FDE</t>
+  </si>
+  <si>
+    <t>##filename##</t>
+  </si>
+  <si>
+    <t>file1</t>
+  </si>
+  <si>
+    <t>file2</t>
+  </si>
+  <si>
+    <t>file3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,15 +120,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -432,18 +464,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C00F07-9D9D-4FB9-8CB2-125007AF4A69}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,59 +492,75 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0.26300000000000001</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>0.26300000000000001</v>
       </c>
       <c r="E2" s="1">
         <v>36872</v>
       </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>124</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.26300000000000001</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>0.26300000000000001</v>
       </c>
       <c r="E3" s="1">
         <v>36873</v>
       </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>125</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.26300000000000001</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="3">
         <v>0.26300000000000001</v>
       </c>
       <c r="E4" s="1">
         <v>36874</v>
       </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>